<commit_message>
fixes and new email feature
fixed param talynM txbrdfw
send mail once task assinged

start of emailing the daily plan.
</commit_message>
<xml_diff>
--- a/lineups/FS - TalynM.TxBrdFW.xlsx
+++ b/lineups/FS - TalynM.TxBrdFW.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Temp</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>SilenceDuration</t>
+  </si>
+  <si>
+    <t>PacketLengthPayload</t>
+  </si>
+  <si>
+    <t>tx_gain_row</t>
   </si>
   <si>
     <t>note</t>
@@ -407,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -415,7 +421,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +470,14 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>-40</v>
       </c>
@@ -511,11 +523,17 @@
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>-40</v>
       </c>
@@ -561,11 +579,17 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>-40</v>
       </c>
@@ -611,11 +635,17 @@
       <c r="O4">
         <v>1</v>
       </c>
-      <c r="P4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>-40</v>
       </c>
@@ -661,11 +691,17 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>-20</v>
       </c>
@@ -711,11 +747,17 @@
       <c r="O6">
         <v>1</v>
       </c>
-      <c r="P6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>-20</v>
       </c>
@@ -761,11 +803,17 @@
       <c r="O7">
         <v>1</v>
       </c>
-      <c r="P7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>-20</v>
       </c>
@@ -811,11 +859,17 @@
       <c r="O8">
         <v>1</v>
       </c>
-      <c r="P8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>-20</v>
       </c>
@@ -861,11 +915,17 @@
       <c r="O9">
         <v>1</v>
       </c>
-      <c r="P9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>100</v>
       </c>
@@ -911,11 +971,17 @@
       <c r="O10">
         <v>2</v>
       </c>
-      <c r="P10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <v>2</v>
+      </c>
+      <c r="R10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>100</v>
       </c>
@@ -961,11 +1027,17 @@
       <c r="O11">
         <v>2</v>
       </c>
-      <c r="P11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>100</v>
       </c>
@@ -1011,11 +1083,17 @@
       <c r="O12">
         <v>2</v>
       </c>
-      <c r="P12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>100</v>
       </c>
@@ -1061,11 +1139,17 @@
       <c r="O13">
         <v>2</v>
       </c>
-      <c r="P13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>105</v>
       </c>
@@ -1111,11 +1195,17 @@
       <c r="O14">
         <v>2</v>
       </c>
-      <c r="P14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>105</v>
       </c>
@@ -1161,11 +1251,17 @@
       <c r="O15">
         <v>2</v>
       </c>
-      <c r="P15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="R15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>105</v>
       </c>
@@ -1211,11 +1307,17 @@
       <c r="O16">
         <v>2</v>
       </c>
-      <c r="P16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>2</v>
+      </c>
+      <c r="R16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>105</v>
       </c>
@@ -1261,8 +1363,14 @@
       <c r="O17">
         <v>2</v>
       </c>
-      <c r="P17" t="s">
-        <v>17</v>
+      <c r="P17">
+        <v>2</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>